<commit_message>
Participant Input MVP, Highlighting V1
</commit_message>
<xml_diff>
--- a/bracket-testing.xlsx
+++ b/bracket-testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nate4\Desktop\Code\Personal\svacketz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86ED14C-70A0-4917-BDEF-6F204122238D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A79081-9109-4DB7-B634-CE84526E2E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F26E6C3D-1F0A-486C-ACE2-5DE3F25AFB5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F26E6C3D-1F0A-486C-ACE2-5DE3F25AFB5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>Total Participants</t>
   </si>
@@ -67,12 +67,30 @@
   <si>
     <t>L</t>
   </si>
+  <si>
+    <t>3 to 1, reverse</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>4 to 1, reverse</t>
+  </si>
+  <si>
+    <t>5 to 1, reverse</t>
+  </si>
+  <si>
+    <t>6 to 1, reverse</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,13 +98,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,9 +145,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9866E087-EF26-436C-AA1F-80CF41421CC3}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>9</v>
       </c>
@@ -735,6 +788,752 @@
       <c r="E17">
         <f>D17*3/4+D16*1/4</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <f>27*3</f>
+        <v>81</v>
+      </c>
+      <c r="D19">
+        <f>C19*1/3</f>
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19" si="4">D19*1/3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <f>C19*2/3</f>
+        <v>54</v>
+      </c>
+      <c r="D20">
+        <f>C20*1/3+D19*2/3</f>
+        <v>36</v>
+      </c>
+      <c r="E20">
+        <f>D20*1/3+E19*2/3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f>C23*3</f>
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <f>E23*3</f>
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <f>H23*3</f>
+        <v>81</v>
+      </c>
+      <c r="K23">
+        <f>81*3</f>
+        <v>243</v>
+      </c>
+      <c r="L23">
+        <f>K23*3</f>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>18</v>
+      </c>
+      <c r="H24">
+        <f>18*2</f>
+        <v>36</v>
+      </c>
+      <c r="I24">
+        <v>54</v>
+      </c>
+      <c r="J24">
+        <v>162</v>
+      </c>
+      <c r="K24">
+        <v>324</v>
+      </c>
+      <c r="L24">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <f>E24+E23*2/3</f>
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25" si="5">F24+F23*2/3</f>
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25" si="6">G24+G23*2/3</f>
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25" si="7">H24+H23*2/3</f>
+        <v>54</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25" si="8">I24+I23*2/3</f>
+        <v>108</v>
+      </c>
+      <c r="J25">
+        <f>J24+J23*2/3</f>
+        <v>162</v>
+      </c>
+      <c r="K25">
+        <f>K24+K23*2/3</f>
+        <v>486</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25" si="9">L24+L23*2/3</f>
+        <v>972</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25" si="10">M24+M23*2/3</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25" si="11">N24+N23*2/3</f>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ref="O25" si="12">O24+O23*2/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" ref="D26:O26" si="13">D23/D25</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="M26" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" ref="E27:K27" si="14">GCD(E23,E24)</f>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="14"/>
+        <v>27</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="14"/>
+        <v>81</v>
+      </c>
+      <c r="L27">
+        <f>GCD(L23,L24)</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <f>F32*4</f>
+        <v>64</v>
+      </c>
+      <c r="I32">
+        <v>256</v>
+      </c>
+      <c r="J32">
+        <f>256*4</f>
+        <v>1024</v>
+      </c>
+      <c r="K32">
+        <f>J32*4</f>
+        <v>4096</v>
+      </c>
+      <c r="M32">
+        <f>K32*4</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>24</v>
+      </c>
+      <c r="G33">
+        <v>48</v>
+      </c>
+      <c r="H33">
+        <v>192</v>
+      </c>
+      <c r="I33">
+        <v>576</v>
+      </c>
+      <c r="J33">
+        <v>1536</v>
+      </c>
+      <c r="K33">
+        <v>3072</v>
+      </c>
+      <c r="L33">
+        <v>12288</v>
+      </c>
+      <c r="M33">
+        <v>36864</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <f>E32*3/4+E33</f>
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:O34" si="15">F32*3/4+F33</f>
+        <v>36</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="15"/>
+        <v>96</v>
+      </c>
+      <c r="H34">
+        <f>H32*3/4+H33</f>
+        <v>192</v>
+      </c>
+      <c r="I34">
+        <f>I32*3/4+I33</f>
+        <v>768</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="15"/>
+        <v>2304</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="15"/>
+        <v>6144</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="15"/>
+        <v>12288</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="15"/>
+        <v>49152</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f>D32/D34</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:O35" si="16">E32/E34</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="16"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="16"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="16"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="16"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="16"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="16"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N35" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f>E34/D34</f>
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:O36" si="17">F34/E34</f>
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="17"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="17"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O36" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f>GCD(D32,D33)</f>
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <f>GCD(E32,E33)</f>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>GCD(F32,F33)</f>
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <f>GCD(G32,G33)</f>
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <f>GCD(I32,I33)</f>
+        <v>64</v>
+      </c>
+      <c r="J37">
+        <f>GCD(J32,J33)</f>
+        <v>512</v>
+      </c>
+      <c r="K37">
+        <f>GCD(K32,K33)</f>
+        <v>1024</v>
+      </c>
+      <c r="M37">
+        <f>GCD(M32,M33)</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <v>125</v>
+      </c>
+      <c r="H40">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>16</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+      <c r="G41">
+        <v>200</v>
+      </c>
+      <c r="H41">
+        <v>500</v>
+      </c>
+      <c r="I41">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <f>E41+E40*4/5</f>
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ref="F42:I42" si="18">F41+F40*4/5</f>
+        <v>80</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="18"/>
+        <v>300</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="18"/>
+        <v>1000</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="18"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" ref="E43:G43" si="19">GCD(E40,E41)</f>
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="H43">
+        <f>GCD(H40,H41)</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <f>E46*6</f>
+        <v>36</v>
+      </c>
+      <c r="G46">
+        <f>F46*6</f>
+        <v>216</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ref="H46:I46" si="20">G46*6</f>
+        <v>1296</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="20"/>
+        <v>7776</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>25</v>
+      </c>
+      <c r="F47">
+        <v>120</v>
+      </c>
+      <c r="G47">
+        <v>540</v>
+      </c>
+      <c r="H47">
+        <v>2160</v>
+      </c>
+      <c r="I47">
+        <v>6480</v>
+      </c>
+      <c r="J47">
+        <v>38880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48">
+        <f>D47+D46*5/6</f>
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:L48" si="21">E47+E46*5/6</f>
+        <v>30</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="21"/>
+        <v>150</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="21"/>
+        <v>720</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="21"/>
+        <v>3240</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="21"/>
+        <v>12960</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="21"/>
+        <v>38880</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" ref="E49:H49" si="22">GCD(E46,E47)</f>
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="22"/>
+        <v>108</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="22"/>
+        <v>432</v>
+      </c>
+      <c r="I49">
+        <f>GCD(I46,I47)</f>
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f>F49/E49</f>
+        <v>12</v>
+      </c>
+      <c r="G50">
+        <f>G49/F49</f>
+        <v>9</v>
+      </c>
+      <c r="H50">
+        <f>H49/G49</f>
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <f>I49/H49</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results Screen Start & Setup Screen Progress
</commit_message>
<xml_diff>
--- a/bracket-testing.xlsx
+++ b/bracket-testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nate4\Desktop\Code\Personal\svacketz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A79081-9109-4DB7-B634-CE84526E2E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F56EAB-B0C8-46F6-97A0-8B5F45885F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F26E6C3D-1F0A-486C-ACE2-5DE3F25AFB5E}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>